<commit_message>
Added graphic file, new version of raport, update all information in markdown
</commit_message>
<xml_diff>
--- a/Project 4 - Power BI dashboard/Data used to this project/51_FIG_World_Championship_2022.xlsx
+++ b/Project 4 - Power BI dashboard/Data used to this project/51_FIG_World_Championship_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/046790313035d56d/Dokumenty/Michał Programuje/Portflio/Project 1 - Data/Clean XLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gymnastics on GitHub!\Gymnastics-on-GitHub\Project 4 - Power BI dashboard\Data used to this project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF117F7E-166C-4EED-91D7-633EBA417BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BADCA9D-9A1C-4DB6-9E40-E2B587384D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Qualification" sheetId="1" r:id="rId1"/>
@@ -43,29 +43,29 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Zapytanie — Table001 (Page 1)" description="Połączenie z zapytaniem „Table001 (Page 1)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1)" description="Połączenie z zapytaniem „Table001 (Page 1)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1)]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Zapytanie — Table001 (Page 1) (2)" description="Połączenie z zapytaniem „Table001 (Page 1) (2)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1) (2)" description="Połączenie z zapytaniem „Table001 (Page 1) (2)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1) (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1) (2)]"/>
   </connection>
-  <connection id="3" keepAlive="1" name="Zapytanie — Table001 (Page 1) (3)" description="Połączenie z zapytaniem „Table001 (Page 1) (3)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1) (3)" description="Połączenie z zapytaniem „Table001 (Page 1) (3)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1) (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1) (3)]"/>
   </connection>
-  <connection id="4" keepAlive="1" name="Zapytanie — Table001 (Page 1) (4)" description="Połączenie z zapytaniem „Table001 (Page 1) (4)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1) (4)" description="Połączenie z zapytaniem „Table001 (Page 1) (4)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1) (4)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1) (4)]"/>
   </connection>
-  <connection id="5" keepAlive="1" name="Zapytanie — Table001 (Page 1) (5)" description="Połączenie z zapytaniem „Table001 (Page 1) (5)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1) (5)" description="Połączenie z zapytaniem „Table001 (Page 1) (5)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1) (5)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1) (5)]"/>
   </connection>
-  <connection id="6" keepAlive="1" name="Zapytanie — Table001 (Page 1) (6)" description="Połączenie z zapytaniem „Table001 (Page 1) (6)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1) (6)" description="Połączenie z zapytaniem „Table001 (Page 1) (6)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1) (6)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1) (6)]"/>
   </connection>
-  <connection id="7" keepAlive="1" name="Zapytanie — Table001 (Page 1) (7)" description="Połączenie z zapytaniem „Table001 (Page 1) (7)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1) (7)" description="Połączenie z zapytaniem „Table001 (Page 1) (7)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1) (7)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1) (7)]"/>
   </connection>
-  <connection id="8" keepAlive="1" name="Zapytanie — Table001 (Page 1-4)" description="Połączenie z zapytaniem „Table001 (Page 1-4)” w skoroszycie." type="5" refreshedVersion="0" background="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" keepAlive="1" name="Zapytanie — Table001 (Page 1-4)" description="Połączenie z zapytaniem „Table001 (Page 1-4)” w skoroszycie." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table001 (Page 1-4)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table001 (Page 1-4)]"/>
   </connection>
 </connections>
@@ -746,10 +746,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -781,11 +781,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1099,14 +1098,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -8985,8 +8987,14 @@
       <c r="D93">
         <v>5.9</v>
       </c>
+      <c r="E93">
+        <v>7</v>
+      </c>
       <c r="F93">
         <v>12.7</v>
+      </c>
+      <c r="G93">
+        <v>-0.2</v>
       </c>
       <c r="H93">
         <v>4.4000000000000004</v>
@@ -9133,8 +9141,14 @@
       <c r="D95">
         <v>5.7</v>
       </c>
+      <c r="E95">
+        <v>6.6</v>
+      </c>
       <c r="F95">
         <v>12.2</v>
+      </c>
+      <c r="G95">
+        <v>-0.1</v>
       </c>
       <c r="H95">
         <v>6.4</v>
@@ -9206,6 +9220,9 @@
       </c>
       <c r="D96">
         <v>5.4</v>
+      </c>
+      <c r="E96">
+        <v>7.9329999999999998</v>
       </c>
       <c r="F96">
         <v>13.333</v>
@@ -9351,7 +9368,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11519,7 +11536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11534,209 +11551,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>191</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>6.2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>8.3330000000000002</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>14.532999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>8.5</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>14.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>6.2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>8.1660000000000004</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>-0.1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>14.266</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>5.6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>8.6329999999999991</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>14.233000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>5.9</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>8.3330000000000002</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>14.233000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5.9</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>14.2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>6.2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>7.1</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>13.3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>6.1</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>12.1</v>
       </c>
     </row>
@@ -11746,7 +11763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11761,209 +11778,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>191</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>6.4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>8.9</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>15.3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>6.3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>8.5660000000000007</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>14.866</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>6.1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>8.6329999999999991</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>14.733000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>197</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>6.3</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>8.2330000000000005</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>14.532999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>6.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>14.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>6.4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>7.133</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>13.532999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>184</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>6.1</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>6.8330000000000002</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>12.933</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>5.7</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>6.8</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>12.5</v>
       </c>
     </row>
@@ -11973,7 +11990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11988,209 +12005,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>191</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>6.3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>8.6329999999999991</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>14.933</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>6.3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>8.5660000000000007</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>14.866</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>6.1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>8.6329999999999991</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>14.733000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>8.6</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>14.6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>6.7</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>7.9</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>14.6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>205</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>8.5329999999999995</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>14.532999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>6.4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>8.0660000000000007</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>14.465999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>8.4329999999999998</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>14.433</v>
       </c>
     </row>
@@ -12200,8 +12217,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
@@ -12271,13 +12288,13 @@
       <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>5.6</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>9.5</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>15</v>
       </c>
       <c r="G2">
@@ -12286,16 +12303,16 @@
       <c r="H2">
         <v>5.6</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>9.5</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>15.1</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>15.05</v>
       </c>
     </row>
@@ -12309,13 +12326,13 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>9.1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>15</v>
       </c>
       <c r="G3">
@@ -12324,16 +12341,16 @@
       <c r="H3">
         <v>5.6</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>14.9</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>14.95</v>
       </c>
     </row>
@@ -12347,13 +12364,13 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>5.6</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>14.8</v>
       </c>
       <c r="G4">
@@ -12362,16 +12379,16 @@
       <c r="H4">
         <v>5.6</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>9.0660000000000007</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>14.666</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>14.733000000000001</v>
       </c>
     </row>
@@ -12385,13 +12402,13 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>5.6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>9.0660000000000007</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>14.666</v>
       </c>
       <c r="G5">
@@ -12400,16 +12417,16 @@
       <c r="H5">
         <v>5.6</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>14.4</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>14.532999999999999</v>
       </c>
     </row>
@@ -12423,13 +12440,13 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>5.6</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>8.7330000000000005</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>14.333</v>
       </c>
       <c r="G6">
@@ -12438,16 +12455,16 @@
       <c r="H6">
         <v>5.6</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>8.9</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>14.5</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>14.416</v>
       </c>
     </row>
@@ -12461,13 +12478,13 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5.6</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>8.8659999999999997</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>14.465999999999999</v>
       </c>
       <c r="G7">
@@ -12476,16 +12493,16 @@
       <c r="H7">
         <v>5.2</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>8.9659999999999993</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>14.166</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>14.316000000000001</v>
       </c>
     </row>
@@ -12499,13 +12516,13 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>5.6</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>8.6660000000000004</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>14.166</v>
       </c>
       <c r="G8">
@@ -12514,16 +12531,16 @@
       <c r="H8">
         <v>4.8</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>9.0329999999999995</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>13.833</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>13.999000000000001</v>
       </c>
     </row>
@@ -12537,13 +12554,13 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>5.6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>14.9</v>
       </c>
       <c r="G9">
@@ -12552,118 +12569,18 @@
       <c r="H9">
         <v>5.2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>8</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>12.9</v>
       </c>
       <c r="K9">
         <v>-0.3</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="L17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12671,7 +12588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12686,209 +12603,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>191</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>6.9</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>9.266</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>16.166</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>6.6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>8.9</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>15.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>6.3</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>9.0660000000000007</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>15.366</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>218</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>6.6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>8.4659999999999993</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>15.066000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>219</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>6.7</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>8.266</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>14.965999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>206</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>6.5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>8.4</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>14.9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>6.4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>8.3330000000000002</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>14.733000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>6.5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>14.7</v>
       </c>
     </row>
@@ -12898,10 +12815,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -12913,209 +12830,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>191</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>6.3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>8.5</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>14.8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>6.4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>14.7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>6</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>8.4659999999999993</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>14.465999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>6.4</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>8.0329999999999995</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>14.433</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>6.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>14.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5.9</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>8.4</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>14.3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>6</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>8.1660000000000004</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>14.166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>5.9</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>7.8659999999999997</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>13.766</v>
       </c>
     </row>

</xml_diff>